<commit_message>
Summary file for input into DC3000 effector heat map
</commit_message>
<xml_diff>
--- a/MM20230601_summary_visual_score_stat_all_positive.xlsx
+++ b/MM20230601_summary_visual_score_stat_all_positive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mende012\Documents\Bioinformatics\Cell_death\Analysis_disease_symptoms_visual_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F403AF6E-4422-4759-B70E-90E243479726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F0C468-9365-4349-8124-31C8EAE89A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="-12645" windowWidth="9600" windowHeight="4905" xr2:uid="{4A0879DF-965F-48AF-852A-00BCE3CACC5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A0879DF-965F-48AF-852A-00BCE3CACC5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="1" r:id="rId1"/>

</xml_diff>